<commit_message>
Add Store test cases
</commit_message>
<xml_diff>
--- a/testData/UserData2.xlsx
+++ b/testData/UserData2.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="19875" windowHeight="7725"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="19875" windowHeight="7725" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="UserData" sheetId="1" r:id="rId1"/>
+    <sheet name="StoreData" sheetId="2" r:id="rId2"/>
+    <sheet name="OrderId" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>test@123</t>
   </si>
@@ -73,6 +74,33 @@
   </si>
   <si>
     <t>UserID</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>PetId</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>shipDate</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>2024-12-03T19:17:38.568Z</t>
+  </si>
+  <si>
+    <t>placed</t>
+  </si>
+  <si>
+    <t>orderId</t>
   </si>
 </sst>
 </file>
@@ -438,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -556,17 +584,173 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1010</v>
+      </c>
+      <c r="B2">
+        <v>1001</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1020</v>
+      </c>
+      <c r="B3">
+        <v>1002</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1030</v>
+      </c>
+      <c r="B4">
+        <v>1003</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>